<commit_message>
Fixed the constant Carousell bugs (hopefully) and added colour to Excel sheet. Almost done with project
</commit_message>
<xml_diff>
--- a/lego_comparison.xlsx
+++ b/lego_comparison.xlsx
@@ -26,12 +26,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEB9C"/>
+        <bgColor rgb="00FFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +64,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,253 +473,343 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>lego cmf heroic knight (71000) medieval castle</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>35</v>
+          <t>lego creator 30688</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>71000</t>
+          <t>30688</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>15.4</v>
+        <v>5.63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>lego 30678 minion's jetboard</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>10</v>
+          <t>lego marvel 76261</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>150</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>30678</t>
+          <t>76261</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>6.3</v>
+        <v>99.86</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>lego city stuntz 60309</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>10</v>
+          <t>lego system 1252 shell tanker truck</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>70</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>60309</t>
+          <t>1252</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8.67</v>
+        <v>58.21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>lego 40355 year of the rat</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>28</v>
+          <t>lego 11033 classic 1800pcs</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>40355</t>
+          <t>11033</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>22.18</v>
+        <v>87.06</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>lego 10714 board</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>10</v>
+          <t>lego architecture london great britain 21034</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10714</t>
+          <t>21034</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8.44</v>
+        <v>32.49</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>lego marvel the punisher from 76178 the daily bugle</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>50</v>
+          <t>lego 76294 (x-men mansion only)</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>140</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>76178</t>
+          <t>76294</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>365.36</v>
+        <v>242.84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>lego friends (41732)</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>220</v>
+          <t>lego technic 42161 lamborghini</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>70</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>41732</t>
+          <t>42161</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>178.04</v>
+        <v>53.58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>lego 75138: hoth attack</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>70</v>
+          <t>lego 60005 fire boat</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>35</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>75138</t>
+          <t>60005</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>89.22</v>
+        <v>72.12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>lego disney king magnifico’s castle 43224 building toy set; detailed castle makes a fun gift for ages 7 and over (613 pieces) christmas gift</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>60</v>
+          <t>clearance sale lego 40529 children's amusement park</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>14.9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>43224</t>
+          <t>40529</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>46.04</v>
+        <v>11.57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[ready stock] lego 43222 disney (100th anniversary) disney castle</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>460</v>
+          <t>lego friends (41732)</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>220</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>43222</t>
+          <t>41732</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>475.51</v>
+        <v>177.79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>lego 75412-1: death trooper and night trooper battle pack (no minifigs or accessories)</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>6</v>
+          <t>lego star wars 4486 &amp; 4487 vintage mini building set from 2003</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>80</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>75412</t>
+          <t>4486</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>26.4</v>
+        <v>27.18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>lego duplo- disney junior mickey’s vacation house 10889</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>80</v>
+          <t>lego 10729</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>35</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10889</t>
+          <t>10729</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>98.25</v>
+        <v>42.47</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>lego 75322 hoth at-st star wars</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
+          <t>lego disney castle 43205</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
         <v>60</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>75322</t>
+          <t>43205</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>68.29000000000001</v>
+        <v>110.76</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>40763 lego children day teddy bear</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>20</v>
+          <t>lego 75372: clone trooper &amp; battle droid battle pack</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>40</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>40763</t>
+          <t>75372</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>20.74</v>
+        <v>20.26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>lego 75337: at-te walker</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>75337</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>120.9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>lego disney king magnifico’s castle 43224 building toy set; detailed castle makes a fun gift for ages 7 and over (613 pieces) christmas gift</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>43224</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>46.04</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>lego 76023 the tumbler- new in box</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>76023</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>284.56</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>lego 6210 jabba’s sail barge</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>665</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>6210</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>868.96</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>lego 40516 - everyone is awesome</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>40516</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>43.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>